<commit_message>
machine learning -> supervised learning -> regression -> Regression:Linear Equation
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -436,12 +436,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>place</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -451,14 +451,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr">
         <is>
           <t>x</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>a</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -466,14 +462,10 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
         <is>
           <t>y</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>b</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -481,14 +473,10 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
         <is>
           <t>z</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>c</t>
         </is>
       </c>
       <c r="C4" t="n">

</xml_diff>